<commit_message>
Added DevHub to j_thomas
</commit_message>
<xml_diff>
--- a/udc/excel/iportal_users.xlsx
+++ b/udc/excel/iportal_users.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16729"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\iPortal\udc\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22515" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22512" windowHeight="12432" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="47">
   <si>
     <t>userid</t>
   </si>
@@ -158,12 +158,15 @@
   </si>
   <si>
     <t>iPortal</t>
+  </si>
+  <si>
+    <t>DevHub</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -777,23 +780,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -829,23 +815,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1004,13 +973,13 @@
       <selection activeCell="A2" sqref="A2:A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1018,7 +987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1026,7 +995,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1034,7 +1003,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1042,7 +1011,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1050,7 +1019,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -1058,7 +1027,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1066,7 +1035,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1074,7 +1043,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1082,7 +1051,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1090,7 +1059,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1105,20 +1074,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C66"/>
+  <dimension ref="A1:C67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58:C66"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="21.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1129,7 +1098,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1140,7 +1109,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1151,7 +1120,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1162,7 +1131,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1173,7 +1142,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1184,7 +1153,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1195,7 +1164,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1206,7 +1175,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1217,7 +1186,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1228,7 +1197,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1239,7 +1208,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -1250,7 +1219,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1261,7 +1230,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -1272,7 +1241,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -1283,7 +1252,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1294,7 +1263,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -1305,7 +1274,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1316,7 +1285,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -1327,7 +1296,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -1338,7 +1307,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -1349,7 +1318,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -1360,7 +1329,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -1371,7 +1340,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1382,7 +1351,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1393,7 +1362,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1404,7 +1373,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1415,7 +1384,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -1426,7 +1395,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1437,7 +1406,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1448,7 +1417,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>28</v>
       </c>
@@ -1459,7 +1428,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>12</v>
       </c>
@@ -1470,7 +1439,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>12</v>
       </c>
@@ -1481,7 +1450,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -1492,7 +1461,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>2</v>
       </c>
@@ -1503,7 +1472,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>4</v>
       </c>
@@ -1514,7 +1483,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>6</v>
       </c>
@@ -1525,7 +1494,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>8</v>
       </c>
@@ -1536,7 +1505,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>22</v>
       </c>
@@ -1547,7 +1516,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>10</v>
       </c>
@@ -1558,7 +1527,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>24</v>
       </c>
@@ -1569,7 +1538,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>26</v>
       </c>
@@ -1580,7 +1549,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>28</v>
       </c>
@@ -1591,7 +1560,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>12</v>
       </c>
@@ -1602,7 +1571,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>2</v>
       </c>
@@ -1613,7 +1582,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>4</v>
       </c>
@@ -1624,7 +1593,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>6</v>
       </c>
@@ -1635,7 +1604,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>8</v>
       </c>
@@ -1646,7 +1615,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>22</v>
       </c>
@@ -1657,7 +1626,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>10</v>
       </c>
@@ -1668,7 +1637,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>24</v>
       </c>
@@ -1679,7 +1648,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>26</v>
       </c>
@@ -1690,7 +1659,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>28</v>
       </c>
@@ -1701,7 +1670,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>12</v>
       </c>
@@ -1712,7 +1681,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>2</v>
       </c>
@@ -1723,7 +1692,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>4</v>
       </c>
@@ -1734,20 +1703,20 @@
         <v>43</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
+        <v>4</v>
+      </c>
+      <c r="B57" t="s">
+        <v>41</v>
+      </c>
+      <c r="C57" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
         <v>2</v>
-      </c>
-      <c r="B57" t="s">
-        <v>44</v>
-      </c>
-      <c r="C57" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>4</v>
       </c>
       <c r="B58" t="s">
         <v>44</v>
@@ -1756,9 +1725,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B59" t="s">
         <v>44</v>
@@ -1767,9 +1736,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B60" t="s">
         <v>44</v>
@@ -1778,9 +1747,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B61" t="s">
         <v>44</v>
@@ -1789,9 +1758,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B62" t="s">
         <v>44</v>
@@ -1800,9 +1769,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="B63" t="s">
         <v>44</v>
@@ -1811,9 +1780,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B64" t="s">
         <v>44</v>
@@ -1822,9 +1791,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B65" t="s">
         <v>44</v>
@@ -1833,14 +1802,25 @@
         <v>45</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="B66" t="s">
         <v>44</v>
       </c>
       <c r="C66" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>12</v>
+      </c>
+      <c r="B67" t="s">
+        <v>44</v>
+      </c>
+      <c r="C67" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed reference to Dev Hub
</commit_message>
<xml_diff>
--- a/udc/excel/iportal_users.xlsx
+++ b/udc/excel/iportal_users.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="46">
   <si>
     <t>userid</t>
   </si>
@@ -158,9 +158,6 @@
   </si>
   <si>
     <t>iPortal</t>
-  </si>
-  <si>
-    <t>DevHub</t>
   </si>
 </sst>
 </file>
@@ -1074,10 +1071,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C67"/>
+  <dimension ref="A1:C66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+      <selection activeCell="A57" sqref="A57:XFD57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1705,18 +1702,18 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B57" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C57" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B58" t="s">
         <v>44</v>
@@ -1727,7 +1724,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B59" t="s">
         <v>44</v>
@@ -1738,7 +1735,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B60" t="s">
         <v>44</v>
@@ -1749,7 +1746,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B61" t="s">
         <v>44</v>
@@ -1760,7 +1757,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B62" t="s">
         <v>44</v>
@@ -1771,7 +1768,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="B63" t="s">
         <v>44</v>
@@ -1782,7 +1779,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B64" t="s">
         <v>44</v>
@@ -1793,7 +1790,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B65" t="s">
         <v>44</v>
@@ -1804,23 +1801,12 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="B66" t="s">
         <v>44</v>
       </c>
       <c r="C66" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>12</v>
-      </c>
-      <c r="B67" t="s">
-        <v>44</v>
-      </c>
-      <c r="C67" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated titles for iPortal users
</commit_message>
<xml_diff>
--- a/udc/excel/iportal_users.xlsx
+++ b/udc/excel/iportal_users.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\iPortal\udc\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="55">
   <si>
     <t>userid</t>
   </si>
@@ -142,9 +142,6 @@
     <t>title</t>
   </si>
   <si>
-    <t>TBD</t>
-  </si>
-  <si>
     <t>app</t>
   </si>
   <si>
@@ -158,6 +155,36 @@
   </si>
   <si>
     <t>iPortal</t>
+  </si>
+  <si>
+    <t>BI Administrator</t>
+  </si>
+  <si>
+    <t>BI Developer</t>
+  </si>
+  <si>
+    <t>SR. BI Developr</t>
+  </si>
+  <si>
+    <t>BI Analyst</t>
+  </si>
+  <si>
+    <t>Data Analyst</t>
+  </si>
+  <si>
+    <t>Marketing Analyst</t>
+  </si>
+  <si>
+    <t>Sales Operations Lead</t>
+  </si>
+  <si>
+    <t>Financial Analyst</t>
+  </si>
+  <si>
+    <t>VP - Operations</t>
+  </si>
+  <si>
+    <t>Sales Territory Mgr</t>
   </si>
 </sst>
 </file>
@@ -1073,8 +1100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57:XFD57"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1466,7 +1493,7 @@
         <v>39</v>
       </c>
       <c r="C35" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -1477,7 +1504,7 @@
         <v>39</v>
       </c>
       <c r="C36" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
@@ -1488,7 +1515,7 @@
         <v>39</v>
       </c>
       <c r="C37" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
@@ -1499,7 +1526,7 @@
         <v>39</v>
       </c>
       <c r="C38" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -1510,7 +1537,7 @@
         <v>39</v>
       </c>
       <c r="C39" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -1521,7 +1548,7 @@
         <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -1532,7 +1559,7 @@
         <v>39</v>
       </c>
       <c r="C41" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
@@ -1543,7 +1570,7 @@
         <v>39</v>
       </c>
       <c r="C42" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
@@ -1554,7 +1581,7 @@
         <v>39</v>
       </c>
       <c r="C43" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
@@ -1565,7 +1592,7 @@
         <v>39</v>
       </c>
       <c r="C44" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
@@ -1573,10 +1600,10 @@
         <v>2</v>
       </c>
       <c r="B45" t="s">
+        <v>40</v>
+      </c>
+      <c r="C45" t="s">
         <v>41</v>
-      </c>
-      <c r="C45" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
@@ -1584,10 +1611,10 @@
         <v>4</v>
       </c>
       <c r="B46" t="s">
+        <v>40</v>
+      </c>
+      <c r="C46" t="s">
         <v>41</v>
-      </c>
-      <c r="C46" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
@@ -1595,10 +1622,10 @@
         <v>6</v>
       </c>
       <c r="B47" t="s">
+        <v>40</v>
+      </c>
+      <c r="C47" t="s">
         <v>41</v>
-      </c>
-      <c r="C47" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
@@ -1606,10 +1633,10 @@
         <v>8</v>
       </c>
       <c r="B48" t="s">
+        <v>40</v>
+      </c>
+      <c r="C48" t="s">
         <v>41</v>
-      </c>
-      <c r="C48" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
@@ -1617,10 +1644,10 @@
         <v>22</v>
       </c>
       <c r="B49" t="s">
+        <v>40</v>
+      </c>
+      <c r="C49" t="s">
         <v>41</v>
-      </c>
-      <c r="C49" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
@@ -1628,10 +1655,10 @@
         <v>10</v>
       </c>
       <c r="B50" t="s">
+        <v>40</v>
+      </c>
+      <c r="C50" t="s">
         <v>41</v>
-      </c>
-      <c r="C50" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
@@ -1639,10 +1666,10 @@
         <v>24</v>
       </c>
       <c r="B51" t="s">
+        <v>40</v>
+      </c>
+      <c r="C51" t="s">
         <v>41</v>
-      </c>
-      <c r="C51" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
@@ -1650,10 +1677,10 @@
         <v>26</v>
       </c>
       <c r="B52" t="s">
+        <v>40</v>
+      </c>
+      <c r="C52" t="s">
         <v>41</v>
-      </c>
-      <c r="C52" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
@@ -1661,10 +1688,10 @@
         <v>28</v>
       </c>
       <c r="B53" t="s">
+        <v>40</v>
+      </c>
+      <c r="C53" t="s">
         <v>41</v>
-      </c>
-      <c r="C53" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
@@ -1672,10 +1699,10 @@
         <v>12</v>
       </c>
       <c r="B54" t="s">
+        <v>40</v>
+      </c>
+      <c r="C54" t="s">
         <v>41</v>
-      </c>
-      <c r="C54" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
@@ -1683,10 +1710,10 @@
         <v>2</v>
       </c>
       <c r="B55" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C55" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
@@ -1694,10 +1721,10 @@
         <v>4</v>
       </c>
       <c r="B56" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C56" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
@@ -1705,10 +1732,10 @@
         <v>2</v>
       </c>
       <c r="B57" t="s">
+        <v>43</v>
+      </c>
+      <c r="C57" t="s">
         <v>44</v>
-      </c>
-      <c r="C57" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
@@ -1716,10 +1743,10 @@
         <v>4</v>
       </c>
       <c r="B58" t="s">
+        <v>43</v>
+      </c>
+      <c r="C58" t="s">
         <v>44</v>
-      </c>
-      <c r="C58" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
@@ -1727,10 +1754,10 @@
         <v>6</v>
       </c>
       <c r="B59" t="s">
+        <v>43</v>
+      </c>
+      <c r="C59" t="s">
         <v>44</v>
-      </c>
-      <c r="C59" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
@@ -1738,10 +1765,10 @@
         <v>8</v>
       </c>
       <c r="B60" t="s">
+        <v>43</v>
+      </c>
+      <c r="C60" t="s">
         <v>44</v>
-      </c>
-      <c r="C60" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
@@ -1749,10 +1776,10 @@
         <v>22</v>
       </c>
       <c r="B61" t="s">
+        <v>43</v>
+      </c>
+      <c r="C61" t="s">
         <v>44</v>
-      </c>
-      <c r="C61" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
@@ -1760,10 +1787,10 @@
         <v>10</v>
       </c>
       <c r="B62" t="s">
+        <v>43</v>
+      </c>
+      <c r="C62" t="s">
         <v>44</v>
-      </c>
-      <c r="C62" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
@@ -1771,10 +1798,10 @@
         <v>24</v>
       </c>
       <c r="B63" t="s">
+        <v>43</v>
+      </c>
+      <c r="C63" t="s">
         <v>44</v>
-      </c>
-      <c r="C63" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
@@ -1782,10 +1809,10 @@
         <v>26</v>
       </c>
       <c r="B64" t="s">
+        <v>43</v>
+      </c>
+      <c r="C64" t="s">
         <v>44</v>
-      </c>
-      <c r="C64" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
@@ -1793,10 +1820,10 @@
         <v>28</v>
       </c>
       <c r="B65" t="s">
+        <v>43</v>
+      </c>
+      <c r="C65" t="s">
         <v>44</v>
-      </c>
-      <c r="C65" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
@@ -1804,10 +1831,10 @@
         <v>12</v>
       </c>
       <c r="B66" t="s">
+        <v>43</v>
+      </c>
+      <c r="C66" t="s">
         <v>44</v>
-      </c>
-      <c r="C66" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added images for each user, show/hide feature for user groups, and about page.
</commit_message>
<xml_diff>
--- a/udc/excel/iportal_users.xlsx
+++ b/udc/excel/iportal_users.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="66">
   <si>
     <t>userid</t>
   </si>
@@ -185,6 +185,39 @@
   </si>
   <si>
     <t>Sales Territory Mgr</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>a_wilson.jpg</t>
+  </si>
+  <si>
+    <t>j_thomas.jpg</t>
+  </si>
+  <si>
+    <t>p_harris.jpg</t>
+  </si>
+  <si>
+    <t>j_green.jpg</t>
+  </si>
+  <si>
+    <t>s_bowers.jpg</t>
+  </si>
+  <si>
+    <t>l_denton.jpg</t>
+  </si>
+  <si>
+    <t>a_foster.jpg</t>
+  </si>
+  <si>
+    <t>e_hanson.jpg</t>
+  </si>
+  <si>
+    <t>l_johnson.jpg</t>
+  </si>
+  <si>
+    <t>e_reese.jpg</t>
   </si>
 </sst>
 </file>
@@ -1098,10 +1131,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C66"/>
+  <dimension ref="A1:C76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1837,6 +1870,116 @@
         <v>44</v>
       </c>
     </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>2</v>
+      </c>
+      <c r="B67" t="s">
+        <v>55</v>
+      </c>
+      <c r="C67" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>4</v>
+      </c>
+      <c r="B68" t="s">
+        <v>55</v>
+      </c>
+      <c r="C68" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>6</v>
+      </c>
+      <c r="B69" t="s">
+        <v>55</v>
+      </c>
+      <c r="C69" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>8</v>
+      </c>
+      <c r="B70" t="s">
+        <v>55</v>
+      </c>
+      <c r="C70" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>22</v>
+      </c>
+      <c r="B71" t="s">
+        <v>55</v>
+      </c>
+      <c r="C71" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>10</v>
+      </c>
+      <c r="B72" t="s">
+        <v>55</v>
+      </c>
+      <c r="C72" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>24</v>
+      </c>
+      <c r="B73" t="s">
+        <v>55</v>
+      </c>
+      <c r="C73" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>26</v>
+      </c>
+      <c r="B74" t="s">
+        <v>55</v>
+      </c>
+      <c r="C74" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>28</v>
+      </c>
+      <c r="B75" t="s">
+        <v>55</v>
+      </c>
+      <c r="C75" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>12</v>
+      </c>
+      <c r="B76" t="s">
+        <v>55</v>
+      </c>
+      <c r="C76" t="s">
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add QMC link to Paul Harris
</commit_message>
<xml_diff>
--- a/udc/excel/iportal_users.xlsx
+++ b/udc/excel/iportal_users.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\Qlik\Sense\ServiceDispatcher\Node\iportal\udc\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="66">
   <si>
     <t>userid</t>
   </si>
@@ -1131,10 +1131,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C76"/>
+  <dimension ref="A1:C77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1762,18 +1762,18 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B57" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C57" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B58" t="s">
         <v>43</v>
@@ -1784,7 +1784,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B59" t="s">
         <v>43</v>
@@ -1795,7 +1795,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B60" t="s">
         <v>43</v>
@@ -1806,7 +1806,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B61" t="s">
         <v>43</v>
@@ -1817,7 +1817,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B62" t="s">
         <v>43</v>
@@ -1828,7 +1828,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="B63" t="s">
         <v>43</v>
@@ -1839,7 +1839,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B64" t="s">
         <v>43</v>
@@ -1850,7 +1850,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B65" t="s">
         <v>43</v>
@@ -1861,7 +1861,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="B66" t="s">
         <v>43</v>
@@ -1872,111 +1872,122 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B67" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C67" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B68" t="s">
         <v>55</v>
       </c>
       <c r="C68" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B69" t="s">
         <v>55</v>
       </c>
       <c r="C69" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B70" t="s">
         <v>55</v>
       </c>
       <c r="C70" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B71" t="s">
         <v>55</v>
       </c>
       <c r="C71" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B72" t="s">
         <v>55</v>
       </c>
       <c r="C72" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="B73" t="s">
         <v>55</v>
       </c>
       <c r="C73" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B74" t="s">
         <v>55</v>
       </c>
       <c r="C74" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B75" t="s">
         <v>55</v>
       </c>
       <c r="C75" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="B76" t="s">
         <v>55</v>
       </c>
       <c r="C76" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>12</v>
+      </c>
+      <c r="B77" t="s">
+        <v>55</v>
+      </c>
+      <c r="C77" t="s">
         <v>65</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Layout changes with PinIt routing
</commit_message>
<xml_diff>
--- a/udc/excel/iportal_users.xlsx
+++ b/udc/excel/iportal_users.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\Qlik\Sense\ServiceDispatcher\Node\iportal\udc\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\Qlik\Sense\EAPowerTools\iPortal\udc\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="74">
   <si>
     <t>userid</t>
   </si>
@@ -163,9 +163,6 @@
     <t>BI Developer</t>
   </si>
   <si>
-    <t>SR. BI Developr</t>
-  </si>
-  <si>
     <t>BI Analyst</t>
   </si>
   <si>
@@ -218,12 +215,39 @@
   </si>
   <si>
     <t>e_reese.jpg</t>
+  </si>
+  <si>
+    <t>SR. BI Developer</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>Administrator</t>
+  </si>
+  <si>
+    <t>Team Admin / Developer</t>
+  </si>
+  <si>
+    <t>Consumer</t>
+  </si>
+  <si>
+    <t>Designer</t>
+  </si>
+  <si>
+    <t>Analyst</t>
+  </si>
+  <si>
+    <t>Contributor</t>
+  </si>
+  <si>
+    <t>Executive Consumer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -701,8 +725,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1131,10 +1156,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C77"/>
+  <dimension ref="A1:D87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1548,7 +1573,7 @@
         <v>39</v>
       </c>
       <c r="C37" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
@@ -1559,7 +1584,7 @@
         <v>39</v>
       </c>
       <c r="C38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -1570,7 +1595,7 @@
         <v>39</v>
       </c>
       <c r="C39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -1581,7 +1606,7 @@
         <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -1592,7 +1617,7 @@
         <v>39</v>
       </c>
       <c r="C41" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
@@ -1603,7 +1628,7 @@
         <v>39</v>
       </c>
       <c r="C42" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
@@ -1614,7 +1639,7 @@
         <v>39</v>
       </c>
       <c r="C43" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
@@ -1625,120 +1650,123 @@
         <v>39</v>
       </c>
       <c r="C44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>2</v>
       </c>
-      <c r="B45" t="s">
-        <v>40</v>
-      </c>
-      <c r="C45" t="s">
-        <v>41</v>
+      <c r="B45" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>4</v>
       </c>
-      <c r="B46" t="s">
-        <v>40</v>
-      </c>
-      <c r="C46" t="s">
-        <v>41</v>
+      <c r="B46" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>6</v>
       </c>
-      <c r="B47" t="s">
-        <v>40</v>
-      </c>
-      <c r="C47" t="s">
-        <v>41</v>
+      <c r="B47" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>8</v>
       </c>
-      <c r="B48" t="s">
-        <v>40</v>
-      </c>
-      <c r="C48" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B48" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>22</v>
       </c>
-      <c r="B49" t="s">
-        <v>40</v>
-      </c>
-      <c r="C49" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B49" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D49" s="1"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>10</v>
       </c>
-      <c r="B50" t="s">
-        <v>40</v>
-      </c>
-      <c r="C50" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B50" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D50" s="1"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>24</v>
       </c>
-      <c r="B51" t="s">
-        <v>40</v>
-      </c>
-      <c r="C51" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B51" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D51" s="1"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>26</v>
       </c>
-      <c r="B52" t="s">
-        <v>40</v>
-      </c>
-      <c r="C52" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B52" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>28</v>
       </c>
-      <c r="B53" t="s">
-        <v>40</v>
-      </c>
-      <c r="C53" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B53" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>12</v>
       </c>
-      <c r="B54" t="s">
-        <v>40</v>
-      </c>
-      <c r="C54" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B54" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>2</v>
       </c>
@@ -1746,10 +1774,10 @@
         <v>40</v>
       </c>
       <c r="C55" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>4</v>
       </c>
@@ -1757,10 +1785,10 @@
         <v>40</v>
       </c>
       <c r="C56" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>6</v>
       </c>
@@ -1768,117 +1796,117 @@
         <v>40</v>
       </c>
       <c r="C57" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B58" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C58" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="B59" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C59" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B60" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C60" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B61" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C61" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B62" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C62" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="B63" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C63" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B64" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C64" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="B65" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C65" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="B66" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C66" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B67" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C67" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
@@ -1886,10 +1914,10 @@
         <v>2</v>
       </c>
       <c r="B68" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C68" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
@@ -1897,10 +1925,10 @@
         <v>4</v>
       </c>
       <c r="B69" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C69" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
@@ -1908,10 +1936,10 @@
         <v>6</v>
       </c>
       <c r="B70" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C70" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
@@ -1919,10 +1947,10 @@
         <v>8</v>
       </c>
       <c r="B71" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C71" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
@@ -1930,10 +1958,10 @@
         <v>22</v>
       </c>
       <c r="B72" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C72" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
@@ -1941,10 +1969,10 @@
         <v>10</v>
       </c>
       <c r="B73" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C73" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
@@ -1952,10 +1980,10 @@
         <v>24</v>
       </c>
       <c r="B74" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C74" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
@@ -1963,10 +1991,10 @@
         <v>26</v>
       </c>
       <c r="B75" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C75" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
@@ -1974,10 +2002,10 @@
         <v>28</v>
       </c>
       <c r="B76" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C76" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
@@ -1985,10 +2013,120 @@
         <v>12</v>
       </c>
       <c r="B77" t="s">
+        <v>43</v>
+      </c>
+      <c r="C77" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>2</v>
+      </c>
+      <c r="B78" t="s">
+        <v>54</v>
+      </c>
+      <c r="C78" t="s">
         <v>55</v>
       </c>
-      <c r="C77" t="s">
-        <v>65</v>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>4</v>
+      </c>
+      <c r="B79" t="s">
+        <v>54</v>
+      </c>
+      <c r="C79" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>6</v>
+      </c>
+      <c r="B80" t="s">
+        <v>54</v>
+      </c>
+      <c r="C80" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>8</v>
+      </c>
+      <c r="B81" t="s">
+        <v>54</v>
+      </c>
+      <c r="C81" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>22</v>
+      </c>
+      <c r="B82" t="s">
+        <v>54</v>
+      </c>
+      <c r="C82" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>10</v>
+      </c>
+      <c r="B83" t="s">
+        <v>54</v>
+      </c>
+      <c r="C83" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>24</v>
+      </c>
+      <c r="B84" t="s">
+        <v>54</v>
+      </c>
+      <c r="C84" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>26</v>
+      </c>
+      <c r="B85" t="s">
+        <v>54</v>
+      </c>
+      <c r="C85" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>28</v>
+      </c>
+      <c r="B86" t="s">
+        <v>54</v>
+      </c>
+      <c r="C86" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>12</v>
+      </c>
+      <c r="B87" t="s">
+        <v>54</v>
+      </c>
+      <c r="C87" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Layout changes with PinIt routing"
This reverts commit 7da47df201fdc1cbcf78d2cf5fba122a0a66048b.
</commit_message>
<xml_diff>
--- a/udc/excel/iportal_users.xlsx
+++ b/udc/excel/iportal_users.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\Qlik\Sense\EAPowerTools\iPortal\udc\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\Qlik\Sense\ServiceDispatcher\Node\iportal\udc\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="66">
   <si>
     <t>userid</t>
   </si>
@@ -163,6 +163,9 @@
     <t>BI Developer</t>
   </si>
   <si>
+    <t>SR. BI Developr</t>
+  </si>
+  <si>
     <t>BI Analyst</t>
   </si>
   <si>
@@ -215,39 +218,12 @@
   </si>
   <si>
     <t>e_reese.jpg</t>
-  </si>
-  <si>
-    <t>SR. BI Developer</t>
-  </si>
-  <si>
-    <t>role</t>
-  </si>
-  <si>
-    <t>Administrator</t>
-  </si>
-  <si>
-    <t>Team Admin / Developer</t>
-  </si>
-  <si>
-    <t>Consumer</t>
-  </si>
-  <si>
-    <t>Designer</t>
-  </si>
-  <si>
-    <t>Analyst</t>
-  </si>
-  <si>
-    <t>Contributor</t>
-  </si>
-  <si>
-    <t>Executive Consumer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -725,9 +701,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1156,10 +1131,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D87"/>
+  <dimension ref="A1:C77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1573,7 +1548,7 @@
         <v>39</v>
       </c>
       <c r="C37" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
@@ -1584,7 +1559,7 @@
         <v>39</v>
       </c>
       <c r="C38" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -1595,7 +1570,7 @@
         <v>39</v>
       </c>
       <c r="C39" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -1606,7 +1581,7 @@
         <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -1617,7 +1592,7 @@
         <v>39</v>
       </c>
       <c r="C41" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
@@ -1628,7 +1603,7 @@
         <v>39</v>
       </c>
       <c r="C42" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
@@ -1639,7 +1614,7 @@
         <v>39</v>
       </c>
       <c r="C43" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
@@ -1650,123 +1625,120 @@
         <v>39</v>
       </c>
       <c r="C44" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>2</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>67</v>
+      <c r="B45" t="s">
+        <v>40</v>
+      </c>
+      <c r="C45" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>4</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>68</v>
+      <c r="B46" t="s">
+        <v>40</v>
+      </c>
+      <c r="C46" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>6</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>68</v>
+      <c r="B47" t="s">
+        <v>40</v>
+      </c>
+      <c r="C47" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>8</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>40</v>
+      </c>
+      <c r="C48" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>22</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D49" s="1"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>40</v>
+      </c>
+      <c r="C49" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>10</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D50" s="1"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
+        <v>40</v>
+      </c>
+      <c r="C50" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>24</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D51" s="1"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
+        <v>40</v>
+      </c>
+      <c r="C51" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>26</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
+        <v>40</v>
+      </c>
+      <c r="C52" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>28</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>40</v>
+      </c>
+      <c r="C53" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>12</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>40</v>
+      </c>
+      <c r="C54" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>2</v>
       </c>
@@ -1774,10 +1746,10 @@
         <v>40</v>
       </c>
       <c r="C55" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>4</v>
       </c>
@@ -1785,10 +1757,10 @@
         <v>40</v>
       </c>
       <c r="C56" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>6</v>
       </c>
@@ -1796,117 +1768,117 @@
         <v>40</v>
       </c>
       <c r="C57" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
+        <v>2</v>
+      </c>
+      <c r="B58" t="s">
+        <v>43</v>
+      </c>
+      <c r="C58" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>4</v>
+      </c>
+      <c r="B59" t="s">
+        <v>43</v>
+      </c>
+      <c r="C59" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>6</v>
+      </c>
+      <c r="B60" t="s">
+        <v>43</v>
+      </c>
+      <c r="C60" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
         <v>8</v>
       </c>
-      <c r="B58" t="s">
-        <v>40</v>
-      </c>
-      <c r="C58" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
+      <c r="B61" t="s">
+        <v>43</v>
+      </c>
+      <c r="C61" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
         <v>22</v>
       </c>
-      <c r="B59" t="s">
-        <v>40</v>
-      </c>
-      <c r="C59" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
+      <c r="B62" t="s">
+        <v>43</v>
+      </c>
+      <c r="C62" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
         <v>10</v>
       </c>
-      <c r="B60" t="s">
-        <v>40</v>
-      </c>
-      <c r="C60" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
+      <c r="B63" t="s">
+        <v>43</v>
+      </c>
+      <c r="C63" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
         <v>24</v>
       </c>
-      <c r="B61" t="s">
-        <v>40</v>
-      </c>
-      <c r="C61" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>26</v>
-      </c>
-      <c r="B62" t="s">
-        <v>40</v>
-      </c>
-      <c r="C62" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>28</v>
-      </c>
-      <c r="B63" t="s">
-        <v>40</v>
-      </c>
-      <c r="C63" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>12</v>
-      </c>
       <c r="B64" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C64" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="B65" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C65" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="B66" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C66" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B67" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C67" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
@@ -1914,10 +1886,10 @@
         <v>2</v>
       </c>
       <c r="B68" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="C68" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
@@ -1925,10 +1897,10 @@
         <v>4</v>
       </c>
       <c r="B69" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="C69" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
@@ -1936,10 +1908,10 @@
         <v>6</v>
       </c>
       <c r="B70" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="C70" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
@@ -1947,10 +1919,10 @@
         <v>8</v>
       </c>
       <c r="B71" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="C71" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
@@ -1958,10 +1930,10 @@
         <v>22</v>
       </c>
       <c r="B72" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="C72" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
@@ -1969,10 +1941,10 @@
         <v>10</v>
       </c>
       <c r="B73" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="C73" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
@@ -1980,10 +1952,10 @@
         <v>24</v>
       </c>
       <c r="B74" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="C74" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
@@ -1991,10 +1963,10 @@
         <v>26</v>
       </c>
       <c r="B75" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="C75" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
@@ -2002,10 +1974,10 @@
         <v>28</v>
       </c>
       <c r="B76" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="C76" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
@@ -2013,120 +1985,10 @@
         <v>12</v>
       </c>
       <c r="B77" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="C77" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
-        <v>2</v>
-      </c>
-      <c r="B78" t="s">
-        <v>54</v>
-      </c>
-      <c r="C78" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
-        <v>4</v>
-      </c>
-      <c r="B79" t="s">
-        <v>54</v>
-      </c>
-      <c r="C79" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
-        <v>6</v>
-      </c>
-      <c r="B80" t="s">
-        <v>54</v>
-      </c>
-      <c r="C80" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
-        <v>8</v>
-      </c>
-      <c r="B81" t="s">
-        <v>54</v>
-      </c>
-      <c r="C81" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
-        <v>22</v>
-      </c>
-      <c r="B82" t="s">
-        <v>54</v>
-      </c>
-      <c r="C82" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
-        <v>10</v>
-      </c>
-      <c r="B83" t="s">
-        <v>54</v>
-      </c>
-      <c r="C83" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
-        <v>24</v>
-      </c>
-      <c r="B84" t="s">
-        <v>54</v>
-      </c>
-      <c r="C84" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
-        <v>26</v>
-      </c>
-      <c r="B85" t="s">
-        <v>54</v>
-      </c>
-      <c r="C85" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
-        <v>28</v>
-      </c>
-      <c r="B86" t="s">
-        <v>54</v>
-      </c>
-      <c r="C86" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
-        <v>12</v>
-      </c>
-      <c r="B87" t="s">
-        <v>54</v>
-      </c>
-      <c r="C87" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Revert "Layout changes with PinIt routing""
This reverts commit b3abc6e60a1ace352f50ad90c4d93fbd68452034.
</commit_message>
<xml_diff>
--- a/udc/excel/iportal_users.xlsx
+++ b/udc/excel/iportal_users.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\Qlik\Sense\ServiceDispatcher\Node\iportal\udc\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\Qlik\Sense\EAPowerTools\iPortal\udc\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="74">
   <si>
     <t>userid</t>
   </si>
@@ -163,9 +163,6 @@
     <t>BI Developer</t>
   </si>
   <si>
-    <t>SR. BI Developr</t>
-  </si>
-  <si>
     <t>BI Analyst</t>
   </si>
   <si>
@@ -218,12 +215,39 @@
   </si>
   <si>
     <t>e_reese.jpg</t>
+  </si>
+  <si>
+    <t>SR. BI Developer</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>Administrator</t>
+  </si>
+  <si>
+    <t>Team Admin / Developer</t>
+  </si>
+  <si>
+    <t>Consumer</t>
+  </si>
+  <si>
+    <t>Designer</t>
+  </si>
+  <si>
+    <t>Analyst</t>
+  </si>
+  <si>
+    <t>Contributor</t>
+  </si>
+  <si>
+    <t>Executive Consumer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -701,8 +725,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1131,10 +1156,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C77"/>
+  <dimension ref="A1:D87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1548,7 +1573,7 @@
         <v>39</v>
       </c>
       <c r="C37" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
@@ -1559,7 +1584,7 @@
         <v>39</v>
       </c>
       <c r="C38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -1570,7 +1595,7 @@
         <v>39</v>
       </c>
       <c r="C39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -1581,7 +1606,7 @@
         <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -1592,7 +1617,7 @@
         <v>39</v>
       </c>
       <c r="C41" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
@@ -1603,7 +1628,7 @@
         <v>39</v>
       </c>
       <c r="C42" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
@@ -1614,7 +1639,7 @@
         <v>39</v>
       </c>
       <c r="C43" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
@@ -1625,120 +1650,123 @@
         <v>39</v>
       </c>
       <c r="C44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>2</v>
       </c>
-      <c r="B45" t="s">
-        <v>40</v>
-      </c>
-      <c r="C45" t="s">
-        <v>41</v>
+      <c r="B45" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>4</v>
       </c>
-      <c r="B46" t="s">
-        <v>40</v>
-      </c>
-      <c r="C46" t="s">
-        <v>41</v>
+      <c r="B46" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>6</v>
       </c>
-      <c r="B47" t="s">
-        <v>40</v>
-      </c>
-      <c r="C47" t="s">
-        <v>41</v>
+      <c r="B47" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>8</v>
       </c>
-      <c r="B48" t="s">
-        <v>40</v>
-      </c>
-      <c r="C48" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B48" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>22</v>
       </c>
-      <c r="B49" t="s">
-        <v>40</v>
-      </c>
-      <c r="C49" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B49" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D49" s="1"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>10</v>
       </c>
-      <c r="B50" t="s">
-        <v>40</v>
-      </c>
-      <c r="C50" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B50" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D50" s="1"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>24</v>
       </c>
-      <c r="B51" t="s">
-        <v>40</v>
-      </c>
-      <c r="C51" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B51" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D51" s="1"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>26</v>
       </c>
-      <c r="B52" t="s">
-        <v>40</v>
-      </c>
-      <c r="C52" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B52" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>28</v>
       </c>
-      <c r="B53" t="s">
-        <v>40</v>
-      </c>
-      <c r="C53" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B53" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>12</v>
       </c>
-      <c r="B54" t="s">
-        <v>40</v>
-      </c>
-      <c r="C54" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B54" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>2</v>
       </c>
@@ -1746,10 +1774,10 @@
         <v>40</v>
       </c>
       <c r="C55" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>4</v>
       </c>
@@ -1757,10 +1785,10 @@
         <v>40</v>
       </c>
       <c r="C56" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>6</v>
       </c>
@@ -1768,117 +1796,117 @@
         <v>40</v>
       </c>
       <c r="C57" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B58" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C58" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="B59" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C59" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B60" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C60" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B61" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C61" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B62" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C62" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="B63" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C63" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B64" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C64" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="B65" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C65" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="B66" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C66" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B67" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C67" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
@@ -1886,10 +1914,10 @@
         <v>2</v>
       </c>
       <c r="B68" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C68" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
@@ -1897,10 +1925,10 @@
         <v>4</v>
       </c>
       <c r="B69" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C69" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
@@ -1908,10 +1936,10 @@
         <v>6</v>
       </c>
       <c r="B70" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C70" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
@@ -1919,10 +1947,10 @@
         <v>8</v>
       </c>
       <c r="B71" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C71" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
@@ -1930,10 +1958,10 @@
         <v>22</v>
       </c>
       <c r="B72" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C72" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
@@ -1941,10 +1969,10 @@
         <v>10</v>
       </c>
       <c r="B73" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C73" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
@@ -1952,10 +1980,10 @@
         <v>24</v>
       </c>
       <c r="B74" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C74" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
@@ -1963,10 +1991,10 @@
         <v>26</v>
       </c>
       <c r="B75" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C75" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
@@ -1974,10 +2002,10 @@
         <v>28</v>
       </c>
       <c r="B76" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C76" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
@@ -1985,10 +2013,120 @@
         <v>12</v>
       </c>
       <c r="B77" t="s">
+        <v>43</v>
+      </c>
+      <c r="C77" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>2</v>
+      </c>
+      <c r="B78" t="s">
+        <v>54</v>
+      </c>
+      <c r="C78" t="s">
         <v>55</v>
       </c>
-      <c r="C77" t="s">
-        <v>65</v>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>4</v>
+      </c>
+      <c r="B79" t="s">
+        <v>54</v>
+      </c>
+      <c r="C79" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>6</v>
+      </c>
+      <c r="B80" t="s">
+        <v>54</v>
+      </c>
+      <c r="C80" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>8</v>
+      </c>
+      <c r="B81" t="s">
+        <v>54</v>
+      </c>
+      <c r="C81" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>22</v>
+      </c>
+      <c r="B82" t="s">
+        <v>54</v>
+      </c>
+      <c r="C82" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>10</v>
+      </c>
+      <c r="B83" t="s">
+        <v>54</v>
+      </c>
+      <c r="C83" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>24</v>
+      </c>
+      <c r="B84" t="s">
+        <v>54</v>
+      </c>
+      <c r="C84" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>26</v>
+      </c>
+      <c r="B85" t="s">
+        <v>54</v>
+      </c>
+      <c r="C85" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>28</v>
+      </c>
+      <c r="B86" t="s">
+        <v>54</v>
+      </c>
+      <c r="C86" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>12</v>
+      </c>
+      <c r="B87" t="s">
+        <v>54</v>
+      </c>
+      <c r="C87" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
converted to using csv files and added dynamic way to add entry points
</commit_message>
<xml_diff>
--- a/udc/excel/iportal_users.xlsx
+++ b/udc/excel/iportal_users.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\Qlik\Sense\ServiceDispatcher\Node\iportal\udc\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\My Documents\_Git\iPortal\udc\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22512" windowHeight="12432" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22515" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="68">
   <si>
     <t>userid</t>
   </si>
@@ -218,12 +218,18 @@
   </si>
   <si>
     <t>e_reese.jpg</t>
+  </si>
+  <si>
+    <t>bubba</t>
+  </si>
+  <si>
+    <t>jog</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -837,6 +843,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -872,6 +895,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1024,19 +1064,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1044,7 +1084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1052,7 +1092,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1060,7 +1100,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1068,7 +1108,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1076,7 +1116,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -1084,7 +1124,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1092,7 +1132,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1100,7 +1140,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1108,7 +1148,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1116,12 +1156,28 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1133,18 +1189,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" customWidth="1"/>
-    <col min="3" max="3" width="21.44140625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1155,7 +1211,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1166,7 +1222,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1177,7 +1233,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1188,7 +1244,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1199,7 +1255,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1210,7 +1266,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1221,7 +1277,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1232,7 +1288,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1243,7 +1299,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1254,7 +1310,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1265,7 +1321,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -1276,7 +1332,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1287,7 +1343,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -1298,7 +1354,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -1309,7 +1365,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1320,7 +1376,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -1331,7 +1387,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1342,7 +1398,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -1353,7 +1409,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -1364,7 +1420,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -1375,7 +1431,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -1386,7 +1442,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -1397,7 +1453,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1408,7 +1464,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1419,7 +1475,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1430,7 +1486,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1441,7 +1497,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -1452,7 +1508,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1463,7 +1519,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1474,7 +1530,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>28</v>
       </c>
@@ -1485,7 +1541,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>12</v>
       </c>
@@ -1496,7 +1552,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>12</v>
       </c>
@@ -1507,7 +1563,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -1518,7 +1574,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>2</v>
       </c>
@@ -1529,7 +1585,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>4</v>
       </c>
@@ -1540,7 +1596,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>6</v>
       </c>
@@ -1551,7 +1607,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>8</v>
       </c>
@@ -1562,7 +1618,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>22</v>
       </c>
@@ -1573,7 +1629,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>10</v>
       </c>
@@ -1584,7 +1640,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>24</v>
       </c>
@@ -1595,7 +1651,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>26</v>
       </c>
@@ -1606,7 +1662,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>28</v>
       </c>
@@ -1617,7 +1673,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>12</v>
       </c>
@@ -1628,7 +1684,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>2</v>
       </c>
@@ -1639,7 +1695,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>4</v>
       </c>
@@ -1650,7 +1706,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>6</v>
       </c>
@@ -1661,7 +1717,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>8</v>
       </c>
@@ -1672,7 +1728,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>22</v>
       </c>
@@ -1683,7 +1739,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>10</v>
       </c>
@@ -1694,7 +1750,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>24</v>
       </c>
@@ -1705,7 +1761,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>26</v>
       </c>
@@ -1716,7 +1772,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>28</v>
       </c>
@@ -1727,7 +1783,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>12</v>
       </c>
@@ -1738,7 +1794,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>2</v>
       </c>
@@ -1749,7 +1805,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>4</v>
       </c>
@@ -1760,7 +1816,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>6</v>
       </c>
@@ -1771,7 +1827,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>2</v>
       </c>
@@ -1782,7 +1838,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>4</v>
       </c>
@@ -1793,7 +1849,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>6</v>
       </c>
@@ -1804,7 +1860,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>8</v>
       </c>
@@ -1815,7 +1871,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>22</v>
       </c>
@@ -1826,7 +1882,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>10</v>
       </c>
@@ -1837,7 +1893,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>24</v>
       </c>
@@ -1848,7 +1904,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>26</v>
       </c>
@@ -1859,7 +1915,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>28</v>
       </c>
@@ -1870,7 +1926,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>12</v>
       </c>
@@ -1881,7 +1937,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>2</v>
       </c>
@@ -1892,7 +1948,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>4</v>
       </c>
@@ -1903,7 +1959,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>6</v>
       </c>
@@ -1914,7 +1970,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>8</v>
       </c>
@@ -1925,7 +1981,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>22</v>
       </c>
@@ -1936,7 +1992,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>10</v>
       </c>
@@ -1947,7 +2003,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>24</v>
       </c>
@@ -1958,7 +2014,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>26</v>
       </c>
@@ -1969,7 +2025,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>28</v>
       </c>
@@ -1980,7 +2036,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>12</v>
       </c>

</xml_diff>